<commit_message>
Fixed incorrect elevation value for TB-4
</commit_message>
<xml_diff>
--- a/Data/salt_comm_comp.xlsx
+++ b/Data/salt_comm_comp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5204897_ad_unsw_edu_au2/Documents/Desktop/PhD/Data_analysis/Project/Functional_traits/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="11_91CE3CC78F79A8D366075C52F37BD2726ACCE354" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74ED6CA5-69C0-4592-B4BC-3ABD22D1FEC5}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="11_91CE3CC78F79A8D366075C52F37BD2726ACCE354" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{438578A9-72D1-44AD-9861-EC7EED8B27B8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1:Z1048576"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="AC46" sqref="AC46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4791,7 +4791,7 @@
         <v>4</v>
       </c>
       <c r="AC45">
-        <v>3.129</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="AD45">
         <v>1</v>
@@ -11744,8 +11744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4449B54B-70CB-4CA8-BFAA-AFF1945A2D1A}">
   <dimension ref="A1:AF94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="AC45" sqref="AC45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16148,7 +16148,7 @@
         <v>4</v>
       </c>
       <c r="AC45">
-        <v>3.129</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="AD45">
         <v>1</v>
@@ -23361,8 +23361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD17A0A-8AEF-4B08-A8C0-A0F3553C1AA0}">
   <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="AA45" sqref="AA45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27231,7 +27231,7 @@
         <v>36</v>
       </c>
       <c r="AA45">
-        <v>3.129</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="AB45" s="2">
         <v>11</v>

</xml_diff>

<commit_message>
Changed pseudonames of two grass species from Grass_sp1 and Grass_sp2 to Grass_D and Grass_E in both the functional_traits_combined_data.xlsx and salt_comm_comp.xlsx.
</commit_message>
<xml_diff>
--- a/Data/salt_comm_comp.xlsx
+++ b/Data/salt_comm_comp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5204897_ad_unsw_edu_au2/Documents/Desktop/PhD/Data_analysis/Project/Functional_traits/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="11_91CE3CC78F79A8D366075C52F37BD2726ACCE354" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{438578A9-72D1-44AD-9861-EC7EED8B27B8}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="11_91CE3CC78F79A8D366075C52F37BD2726ACCE354" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF933B89-F67C-4028-BAC2-513115C9CC6B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="49">
   <si>
     <t>Estuary</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>Natural</t>
+  </si>
+  <si>
+    <t>Grass_D</t>
+  </si>
+  <si>
+    <t>Grass_E</t>
   </si>
 </sst>
 </file>
@@ -23361,11 +23367,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD17A0A-8AEF-4B08-A8C0-A0F3553C1AA0}">
   <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="AA45" sqref="AA45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -23408,10 +23418,10 @@
         <v>18</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>21</v>

</xml_diff>